<commit_message>
create excel file without emailid customers
</commit_message>
<xml_diff>
--- a/invalid_emails.xlsx
+++ b/invalid_emails.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -20,7 +20,34 @@
     <t>Email</t>
   </si>
   <si>
+    <t>7771080120987</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>6750080045432</t>
+  </si>
+  <si>
+    <t>1117080008888</t>
+  </si>
+  <si>
+    <t>1117080088888</t>
+  </si>
+  <si>
+    <t>1135088888888</t>
+  </si>
+  <si>
+    <t>1153080077777</t>
+  </si>
+  <si>
+    <t>2020080166666</t>
+  </si>
+  <si>
+    <t>2020080135555</t>
+  </si>
+  <si>
+    <t>2039080022222</t>
   </si>
 </sst>
 </file>
@@ -83,72 +110,72 @@
       <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
+      <c r="B5" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
+      <c r="B6" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
+      <c r="B7" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>2</v>
+        <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
+      <c r="B8" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
+      <c r="B9" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>2</v>
+        <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
+      <c r="B10" t="s" s="0">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>